<commit_message>
local score : .9565, online score : .91935
</commit_message>
<xml_diff>
--- a/Predicted.xlsx
+++ b/Predicted.xlsx
@@ -387,7 +387,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -522,7 +522,7 @@
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:1">
@@ -572,7 +572,7 @@
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:1">
@@ -622,7 +622,7 @@
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:1">
@@ -677,7 +677,7 @@
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:1">
@@ -827,7 +827,7 @@
     </row>
     <row r="90" spans="1:1">
       <c r="A90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:1">
@@ -857,7 +857,7 @@
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:1">
@@ -997,7 +997,7 @@
     </row>
     <row r="124" spans="1:1">
       <c r="A124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:1">
@@ -1102,7 +1102,7 @@
     </row>
     <row r="145" spans="1:1">
       <c r="A145">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:1">
@@ -1382,12 +1382,12 @@
     </row>
     <row r="201" spans="1:1">
       <c r="A201">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:1">
@@ -1417,7 +1417,7 @@
     </row>
     <row r="208" spans="1:1">
       <c r="A208">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:1">
@@ -1487,7 +1487,7 @@
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:1">
@@ -1532,7 +1532,7 @@
     </row>
     <row r="231" spans="1:1">
       <c r="A231">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:1">
@@ -1647,7 +1647,7 @@
     </row>
     <row r="254" spans="1:1">
       <c r="A254">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:1">
@@ -1767,7 +1767,7 @@
     </row>
     <row r="278" spans="1:1">
       <c r="A278">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:1">
@@ -1777,7 +1777,7 @@
     </row>
     <row r="280" spans="1:1">
       <c r="A280">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:1">
@@ -1847,7 +1847,7 @@
     </row>
     <row r="294" spans="1:1">
       <c r="A294">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295" spans="1:1">
@@ -2257,7 +2257,7 @@
     </row>
     <row r="376" spans="1:1">
       <c r="A376">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:1">
@@ -2322,7 +2322,7 @@
     </row>
     <row r="389" spans="1:1">
       <c r="A389">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390" spans="1:1">
@@ -2342,7 +2342,7 @@
     </row>
     <row r="393" spans="1:1">
       <c r="A393">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="394" spans="1:1">
@@ -2657,7 +2657,7 @@
     </row>
     <row r="456" spans="1:1">
       <c r="A456">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="457" spans="1:1">
@@ -2782,7 +2782,7 @@
     </row>
     <row r="481" spans="1:1">
       <c r="A481">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="482" spans="1:1">
@@ -2817,7 +2817,7 @@
     </row>
     <row r="488" spans="1:1">
       <c r="A488">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="489" spans="1:1">
@@ -2892,7 +2892,7 @@
     </row>
     <row r="503" spans="1:1">
       <c r="A503">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="504" spans="1:1">
@@ -2992,7 +2992,7 @@
     </row>
     <row r="523" spans="1:1">
       <c r="A523">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="524" spans="1:1">
@@ -3017,7 +3017,7 @@
     </row>
     <row r="528" spans="1:1">
       <c r="A528">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
96.43 local , leaderborad : 90.
</commit_message>
<xml_diff>
--- a/Predicted.xlsx
+++ b/Predicted.xlsx
@@ -437,7 +437,7 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1">
@@ -622,7 +622,7 @@
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:1">
@@ -637,12 +637,12 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -667,7 +667,7 @@
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:1">
@@ -777,7 +777,7 @@
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:1">
@@ -1157,7 +1157,7 @@
     </row>
     <row r="156" spans="1:1">
       <c r="A156">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:1">
@@ -1667,7 +1667,7 @@
     </row>
     <row r="258" spans="1:1">
       <c r="A258">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259" spans="1:1">
@@ -1767,7 +1767,7 @@
     </row>
     <row r="278" spans="1:1">
       <c r="A278">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="279" spans="1:1">
@@ -2132,7 +2132,7 @@
     </row>
     <row r="351" spans="1:1">
       <c r="A351">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="352" spans="1:1">
@@ -2257,7 +2257,7 @@
     </row>
     <row r="376" spans="1:1">
       <c r="A376">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="377" spans="1:1">
@@ -2782,7 +2782,7 @@
     </row>
     <row r="481" spans="1:1">
       <c r="A481">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="482" spans="1:1">
@@ -2892,7 +2892,7 @@
     </row>
     <row r="503" spans="1:1">
       <c r="A503">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="504" spans="1:1">

</xml_diff>